<commit_message>
ADD SEURAT WRAPPER FUNCTIONS FOR NICHENET and fixes of some vignettes
</commit_message>
<xml_diff>
--- a/vignettes/data_sources.xlsx
+++ b/vignettes/data_sources.xlsx
@@ -15,7 +15,6 @@
     <sheet name="datasource_overview" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -957,22 +956,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" customWidth="1"/>
-    <col min="5" max="5" width="71.140625" customWidth="1"/>
-    <col min="6" max="6" width="44.85546875" customWidth="1"/>
-    <col min="7" max="7" width="71.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="5" max="5" width="71.109375" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" customWidth="1"/>
+    <col min="7" max="7" width="71.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -995,7 +994,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1018,7 +1017,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -1041,7 +1040,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1064,7 +1063,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>43206</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -1347,7 +1346,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -1387,7 +1386,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
@@ -1407,7 +1406,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
@@ -1447,7 +1446,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>54</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>72</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -1530,7 +1529,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -1553,7 +1552,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -1576,7 +1575,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>79</v>
       </c>
@@ -1596,7 +1595,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>79</v>
       </c>
@@ -1616,7 +1615,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
@@ -1636,7 +1635,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>79</v>
       </c>
@@ -1656,7 +1655,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>85</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>85</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>43204</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>89</v>
       </c>
@@ -1719,7 +1718,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>92</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>96</v>
       </c>
@@ -1785,7 +1784,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>96</v>
       </c>
@@ -1805,7 +1804,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
@@ -1825,7 +1824,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>96</v>
       </c>
@@ -1845,7 +1844,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>96</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>96</v>
       </c>
@@ -1885,7 +1884,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>103</v>
       </c>
@@ -1903,7 +1902,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>103</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>103</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>103</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>108</v>
       </c>
@@ -1975,7 +1974,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>108</v>
       </c>
@@ -1993,7 +1992,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>108</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>108</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>113</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>116</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>116</v>
       </c>
@@ -2092,7 +2091,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>120</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>123</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>

</xml_diff>